<commit_message>
fixed some things so it works better with the newer version of the script mainly appfolderpath
</commit_message>
<xml_diff>
--- a/pipelines.xlsx
+++ b/pipelines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\MSIAppFactory-YamlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF70CF3-7B7D-4BE2-B96C-32D71588BDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763AA138-DFE6-42A2-B4D2-78B5C760D0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,6 +33,21 @@
     <t>Pipeline Source 1</t>
   </si>
   <si>
+    <t>Pipeline 2</t>
+  </si>
+  <si>
+    <t>Pipeline Source 2</t>
+  </si>
+  <si>
+    <t>pipeline</t>
+  </si>
+  <si>
+    <t>pipelineSource</t>
+  </si>
+  <si>
+    <t>AppFolderPath</t>
+  </si>
+  <si>
     <r>
       <t>Apps</t>
     </r>
@@ -52,14 +67,8 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>app1.json</t>
-    </r>
-  </si>
-  <si>
-    <t>Pipeline 2</t>
-  </si>
-  <si>
-    <t>Pipeline Source 2</t>
+      <t>App1</t>
+    </r>
   </si>
   <si>
     <r>
@@ -81,17 +90,8 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>app2.json</t>
-    </r>
-  </si>
-  <si>
-    <t>pipeline</t>
-  </si>
-  <si>
-    <t>pipelineSource</t>
-  </si>
-  <si>
-    <t>jsonFile</t>
+      <t>App2</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F4" activeCellId="1" sqref="C3 F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,13 +436,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -453,18 +453,18 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added parameters for the build process as wel as a naming for the pipeline
</commit_message>
<xml_diff>
--- a/pipelines.xlsx
+++ b/pipelines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\MSIAppFactory-YamlGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763AA138-DFE6-42A2-B4D2-78B5C760D0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D715C0-C911-4152-807E-D03CE71FF01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,18 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Pipeline 1</t>
-  </si>
-  <si>
-    <t>Pipeline Source 1</t>
-  </si>
-  <si>
-    <t>Pipeline 2</t>
-  </si>
-  <si>
-    <t>Pipeline Source 2</t>
-  </si>
-  <si>
     <t>pipeline</t>
   </si>
   <si>
@@ -92,6 +80,18 @@
       </rPr>
       <t>App2</t>
     </r>
+  </si>
+  <si>
+    <t>Pipeline_1</t>
+  </si>
+  <si>
+    <t>Pipeline_2</t>
+  </si>
+  <si>
+    <t>Pipeline_Source_1</t>
+  </si>
+  <si>
+    <t>Pipeline_Source_2</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" activeCellId="1" sqref="C3 F4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,35 +436,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>